<commit_message>
Cambios prueba tecnica 16-10-23
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DataFile.xlsx
+++ b/src/test/resources/data/DataFile.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergo\eclipse-workspace\PruebaTecnica\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergo\git\PruebaTecnica\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D74AC72-D095-43F2-A167-66BC588CA24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CBF3F1-0204-482F-8575-4FD3C3F593D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{57FD9A9C-3739-40AC-98DC-1727BACCA774}"/>
   </bookViews>
   <sheets>
-    <sheet name="compensar" sheetId="1" r:id="rId1"/>
+    <sheet name="pruebaTecnica" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,36 +36,117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>TAG</t>
   </si>
   <si>
-    <t>keyTipoDocumento</t>
-  </si>
-  <si>
-    <t>keyDocumento</t>
-  </si>
-  <si>
-    <t>@registrarseEnPagina</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>94090402204_Ser</t>
-  </si>
-  <si>
-    <t>keyClave</t>
-  </si>
-  <si>
-    <t>1013652139</t>
+    <t>keyUserName</t>
+  </si>
+  <si>
+    <t>keyPassword</t>
+  </si>
+  <si>
+    <t>test01</t>
+  </si>
+  <si>
+    <t>Test2023*</t>
+  </si>
+  <si>
+    <t>keyBook1</t>
+  </si>
+  <si>
+    <t>Programming JavaScript</t>
+  </si>
+  <si>
+    <t>keyBook2</t>
+  </si>
+  <si>
+    <t>Understanding ECMAScript 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @PruebaTecnicaPunto1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @PruebaTecnicaPunto2</t>
+  </si>
+  <si>
+    <t>test02</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>keyLastName</t>
+  </si>
+  <si>
+    <t>Prueba01</t>
+  </si>
+  <si>
+    <t>keyEmail</t>
+  </si>
+  <si>
+    <t>prueba@yopmail.com</t>
+  </si>
+  <si>
+    <t>keyGender</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>keyMobile</t>
+  </si>
+  <si>
+    <t>3004441234</t>
+  </si>
+  <si>
+    <t>keyBirthDate</t>
+  </si>
+  <si>
+    <t>27 Sep 2000</t>
+  </si>
+  <si>
+    <t>keySubjects</t>
+  </si>
+  <si>
+    <t>keyHobbies</t>
+  </si>
+  <si>
+    <t>keyCurrentAddress</t>
+  </si>
+  <si>
+    <t>keyState</t>
+  </si>
+  <si>
+    <t>keyCity</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>karnal</t>
+  </si>
+  <si>
+    <t>Autopista Norte al oriente</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>keyFirstName</t>
+  </si>
+  <si>
+    <t>Computer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="d\ mmm\ yyyy"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -111,12 +192,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -432,22 +515,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165510E6-AC97-4009-A097-81F90CC51CC3}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="6" max="7" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -458,25 +541,147 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="3"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>